<commit_message>
Implemented unclaim screen functionality
</commit_message>
<xml_diff>
--- a/sources/Branche_Input.xlsx
+++ b/sources/Branche_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antig\Documents\ERA\Wice_Administration\ERA_Automation_Tool\Tool_Executable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CVR\PAT\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A90D2A0-D14E-4E65-B3BF-122BE4F1072A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B65D5-10AA-4B9F-B164-E62504A6D6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28908" yWindow="-2340" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Branche_l</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Freiberufliche, wissenschaftliche und technische Dienstleistungen</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -141,12 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -165,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -311,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -453,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -480,239 +484,244 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>4000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>4000</v>
       </c>
-      <c r="B3">
-        <v>10000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>4000</v>
+      </c>
+      <c r="B4">
         <v>10000</v>
       </c>
-      <c r="B4">
-        <v>34000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
         <v>34000</v>
       </c>
-      <c r="B5">
-        <v>36000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>34000</v>
+      </c>
+      <c r="B6">
         <v>36000</v>
       </c>
-      <c r="B6">
-        <v>40000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>36000</v>
+      </c>
+      <c r="B7">
         <v>40000</v>
       </c>
-      <c r="B7">
-        <v>44000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>40000</v>
+      </c>
+      <c r="B8">
         <v>44000</v>
       </c>
-      <c r="B8">
-        <v>48000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>44000</v>
+      </c>
+      <c r="B9">
         <v>48000</v>
       </c>
-      <c r="B9">
-        <v>54000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>48000</v>
+      </c>
+      <c r="B10">
         <v>54000</v>
       </c>
-      <c r="B10">
-        <v>57000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>54000</v>
+      </c>
+      <c r="B11">
         <v>57000</v>
       </c>
-      <c r="B11">
-        <v>64000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>57000</v>
+      </c>
+      <c r="B12">
         <v>64000</v>
       </c>
-      <c r="B12">
-        <v>67000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>64000</v>
+      </c>
+      <c r="B13">
         <v>67000</v>
       </c>
-      <c r="B13">
-        <v>69000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>67000</v>
+      </c>
+      <c r="B14">
         <v>69000</v>
       </c>
-      <c r="B14">
-        <v>76000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
+        <v>69000</v>
+      </c>
+      <c r="B15">
         <v>76000</v>
       </c>
-      <c r="B15">
-        <v>83000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
+        <v>76000</v>
+      </c>
+      <c r="B16">
         <v>83000</v>
       </c>
-      <c r="B16">
-        <v>85000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>83000</v>
+      </c>
+      <c r="B17">
         <v>85000</v>
       </c>
-      <c r="B17">
-        <v>86000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
+        <v>85000</v>
+      </c>
+      <c r="B18">
         <v>86000</v>
       </c>
-      <c r="B18">
-        <v>90000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
+        <v>86000</v>
+      </c>
+      <c r="B19">
         <v>90000</v>
       </c>
-      <c r="B19">
-        <v>94000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
+        <v>90000</v>
+      </c>
+      <c r="B20">
         <v>94000</v>
       </c>
-      <c r="B20">
-        <v>97000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
+      <c r="C20" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>94000</v>
+      </c>
+      <c r="B21">
         <v>97000</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>97000</v>
+      </c>
+      <c r="B22">
         <v>99000</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>99000</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>100000</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>